<commit_message>
kavya changes for the commit
</commit_message>
<xml_diff>
--- a/PACTIV/src/test/resources/testdata/Execution_Configuration.xlsx
+++ b/PACTIV/src/test/resources/testdata/Execution_Configuration.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="56">
   <si>
     <t>Execute</t>
   </si>
@@ -56,364 +56,130 @@
     <t>Chrome</t>
   </si>
   <si>
-    <t>User logins to the application with Incorrect Credentials</t>
-  </si>
-  <si>
     <t>MOORESVILLE</t>
   </si>
   <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>Successful log into Pactiv application with Valid Credentials</t>
+    <t>AutomationTestScriptName</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>FloaterTest</t>
+  </si>
+  <si>
+    <t>line</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>Verify the ProductionTracking Data</t>
+  </si>
+  <si>
+    <t>SupervisorTest</t>
+  </si>
+  <si>
+    <t>test123456</t>
+  </si>
+  <si>
+    <t>PlantManagerTest</t>
+  </si>
+  <si>
+    <t>Line1</t>
+  </si>
+  <si>
+    <t>MaintenanceTest</t>
+  </si>
+  <si>
+    <t>MaterialHandlerTest</t>
+  </si>
+  <si>
+    <t>Verify the Headers for Floater</t>
+  </si>
+  <si>
+    <t>Tags</t>
+  </si>
+  <si>
+    <t>Successful log into Moursville application with Valid Credentials</t>
+  </si>
+  <si>
+    <t>Verify the Mooresville PlantView data</t>
+  </si>
+  <si>
+    <t>Successful log into Moursville application with EOL Credentials</t>
+  </si>
+  <si>
+    <t>EOLUser</t>
+  </si>
+  <si>
+    <t>Verify the expand icon navigation On Alarms section in Material Control View</t>
+  </si>
+  <si>
+    <t>Verify user is able to navigate between lines in Material Control View</t>
+  </si>
+  <si>
+    <t>Verify the asset details on each line in Material Control View</t>
+  </si>
+  <si>
+    <t>Verify the details on the Notifications Page</t>
+  </si>
+  <si>
+    <t>Verify the alarm widget data on Mooresville plant view</t>
+  </si>
+  <si>
+    <t>Verify the Navigation to Activity log Mooresville PlantView data</t>
+  </si>
+  <si>
+    <t>Verify the Plant OEE value</t>
+  </si>
+  <si>
+    <t>Verify Supervisor to submit the report</t>
+  </si>
+  <si>
+    <t>Successful log into Production Tracking Tool with Valid Credentials</t>
+  </si>
+  <si>
+    <t>ProductName</t>
+  </si>
+  <si>
+    <t>OrderNumber</t>
+  </si>
+  <si>
+    <t>GoldenOutputPerHour</t>
+  </si>
+  <si>
+    <t>StandardOutputPerHour</t>
+  </si>
+  <si>
+    <t>Totalnumberofcases</t>
+  </si>
+  <si>
+    <t>CPM</t>
+  </si>
+  <si>
+    <t>CaseWeight</t>
+  </si>
+  <si>
+    <t>TableSize</t>
+  </si>
+  <si>
+    <t>xyz</t>
+  </si>
+  <si>
+    <t>flag</t>
   </si>
   <si>
     <t>No</t>
   </si>
   <si>
-    <t>AutomationTestScriptName</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>FloaterTest</t>
-  </si>
-  <si>
-    <t>line</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>Verify the ProductionTracking Data</t>
-  </si>
-  <si>
-    <t>SupervisorTest</t>
-  </si>
-  <si>
-    <t>test123456</t>
-  </si>
-  <si>
-    <t>PlantManagerTest</t>
-  </si>
-  <si>
-    <t>Verify the data on Control Tower Page for ProductionInsights</t>
-  </si>
-  <si>
-    <t>Extruder</t>
-  </si>
-  <si>
-    <t>asset</t>
-  </si>
-  <si>
-    <t>User verify the Extruder2B data on the Asset Detailed View</t>
-  </si>
-  <si>
-    <t>Trim Press</t>
-  </si>
-  <si>
-    <t>User verify the TrimPress1 data on the Asset Detailed View</t>
-  </si>
-  <si>
-    <t>LINE 15</t>
-  </si>
-  <si>
-    <t>TrimPress15</t>
-  </si>
-  <si>
-    <t>Line15</t>
-  </si>
-  <si>
-    <t>HaulOff15</t>
-  </si>
-  <si>
-    <t>Haul Off</t>
-  </si>
-  <si>
-    <t>Extruder15B</t>
-  </si>
-  <si>
-    <t>Thermoformer15</t>
-  </si>
-  <si>
-    <t>Thermoformer</t>
-  </si>
-  <si>
-    <t>Blender15B</t>
-  </si>
-  <si>
-    <t>Blender</t>
-  </si>
-  <si>
-    <t>Line</t>
-  </si>
-  <si>
-    <t>assetName</t>
-  </si>
-  <si>
-    <t>User verify the data on the Asset Detailed View</t>
-  </si>
-  <si>
-    <t>Verify the data on Line Assignment Page</t>
-  </si>
-  <si>
-    <t>User verify the Extruder13B data on the Asset Detailed View for staging environment</t>
-  </si>
-  <si>
-    <t>Extruder1B</t>
-  </si>
-  <si>
-    <t>Line1</t>
-  </si>
-  <si>
-    <t>assetname</t>
-  </si>
-  <si>
-    <t>User verify the data on the Asset Detailed View for all assets</t>
-  </si>
-  <si>
-    <t>MaintenanceTest</t>
-  </si>
-  <si>
-    <t>User verify the Extruder13B data on the Asset Detailed View</t>
-  </si>
-  <si>
-    <t>Verify the data on Control Tower Page</t>
-  </si>
-  <si>
-    <t>ProcessSheet_Line3</t>
-  </si>
-  <si>
-    <t>Test_3</t>
-  </si>
-  <si>
-    <t>LINE 3</t>
-  </si>
-  <si>
-    <t>ProcessSheet_Line2</t>
-  </si>
-  <si>
-    <t>Test_2</t>
-  </si>
-  <si>
-    <t>LINE 2</t>
-  </si>
-  <si>
-    <t>processSheet</t>
-  </si>
-  <si>
-    <t>product</t>
-  </si>
-  <si>
-    <t>Upload the Process Sheet after renaming the Product Name</t>
-  </si>
-  <si>
-    <t>ProcessSheet_Line16</t>
-  </si>
-  <si>
-    <t>LINE 18</t>
-  </si>
-  <si>
-    <t>ProcessSheet_Line18</t>
-  </si>
-  <si>
-    <t>LINE 16</t>
-  </si>
-  <si>
-    <t>ProcessSheet_Line14</t>
-  </si>
-  <si>
-    <t>ProcessSheet_Line15</t>
-  </si>
-  <si>
-    <t>LINE 14</t>
-  </si>
-  <si>
-    <t>ProcessSheet_Line11</t>
-  </si>
-  <si>
-    <t>LINE 12</t>
-  </si>
-  <si>
-    <t>ProcessSheet_Line12</t>
-  </si>
-  <si>
-    <t>LINE 11</t>
-  </si>
-  <si>
-    <t>ProcessSheet_Line8</t>
-  </si>
-  <si>
-    <t>LINE 10</t>
-  </si>
-  <si>
-    <t>ProcessSheet_Line10</t>
-  </si>
-  <si>
-    <t>LINE 8</t>
-  </si>
-  <si>
-    <t>ProcessSheet_Line4</t>
-  </si>
-  <si>
-    <t>LINE 6</t>
-  </si>
-  <si>
-    <t>ProcessSheet_Line6</t>
-  </si>
-  <si>
-    <t>LINE 4</t>
-  </si>
-  <si>
-    <t>Upload the Process Sheet and verify the incorrect file upload message</t>
-  </si>
-  <si>
-    <t>Verify the No file error message</t>
-  </si>
-  <si>
-    <t>Upload the Process Sheet and verify the incorrect file message</t>
-  </si>
-  <si>
-    <t>Upload the Process Sheet and verify the duplicate file message</t>
-  </si>
-  <si>
-    <t>Verify User is able to submit the report</t>
-  </si>
-  <si>
-    <t>Upload the Process Sheet after renaming the files</t>
-  </si>
-  <si>
-    <t>User verify the data on the Line View</t>
-  </si>
-  <si>
-    <t>MaterialHandlerTest</t>
-  </si>
-  <si>
-    <t>Verify the Headers for MaterialHandler</t>
-  </si>
-  <si>
-    <t>Verify the Headers for Floater</t>
-  </si>
-  <si>
-    <t>Verify the Headers for Maintenance</t>
-  </si>
-  <si>
-    <t>Verify the Headers for Supervisor</t>
-  </si>
-  <si>
-    <t>Verify the Headers for PlantManager</t>
-  </si>
-  <si>
-    <t>Verify the PlantView data</t>
-  </si>
-  <si>
-    <t>18/18</t>
-  </si>
-  <si>
-    <t>Maintenance</t>
-  </si>
-  <si>
-    <t>Justin Baldoni</t>
-  </si>
-  <si>
-    <t>ChosenLines</t>
-  </si>
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>RoleLeadership</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Verify Maintenance User Profile Page</t>
-  </si>
-  <si>
-    <t>02/18</t>
-  </si>
-  <si>
-    <t>00/18</t>
-  </si>
-  <si>
-    <t>EOH</t>
-  </si>
-  <si>
-    <t>John Doe</t>
-  </si>
-  <si>
-    <t>Verify MaterialHandler User Profile Page</t>
-  </si>
-  <si>
-    <t>03/18</t>
-  </si>
-  <si>
-    <t>Floater</t>
-  </si>
-  <si>
-    <t>Edmundu</t>
-  </si>
-  <si>
-    <t>Verify Floater User Profile Page</t>
-  </si>
-  <si>
-    <t>Supervisor</t>
-  </si>
-  <si>
-    <t>Rob</t>
-  </si>
-  <si>
-    <t>Verify Supervisor User Profile Page</t>
-  </si>
-  <si>
-    <t>Leadership</t>
-  </si>
-  <si>
-    <t>Christine</t>
-  </si>
-  <si>
-    <t>Verify PlantManager User Profile Page</t>
-  </si>
-  <si>
-    <t>Upload the Process Sheet</t>
-  </si>
-  <si>
-    <t>Vista de control de materiales</t>
-  </si>
-  <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>Navigate to MaterialHandler Home Page and Logout</t>
-  </si>
-  <si>
-    <t>Bridgeview Plant View</t>
-  </si>
-  <si>
-    <t>Navigate to Home Page and Logout</t>
-  </si>
-  <si>
-    <t>gfhhfh</t>
-  </si>
-  <si>
-    <t>fgfhfh</t>
-  </si>
-  <si>
-    <t>hhjfj</t>
-  </si>
-  <si>
-    <t>test123</t>
-  </si>
-  <si>
-    <t>flag</t>
-  </si>
-  <si>
-    <t>Tags</t>
+    <t>CasesperPallet</t>
   </si>
   <si>
     <t>SmokeTests</t>
@@ -526,9 +292,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -847,7 +611,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
+      <selection pane="bottomLeft" activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -859,7 +623,7 @@
     <col min="5" max="5" width="29.140625" style="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="29.140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="44.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="36.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="54.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="13.7109375" customWidth="1"/>
     <col min="11" max="11" width="12.42578125" customWidth="1"/>
   </cols>
@@ -895,13 +659,13 @@
         <v>1</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>132</v>
+        <v>29</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>0</v>
@@ -919,20 +683,20 @@
         <v>1</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4" t="s">
-        <v>133</v>
+        <v>55</v>
       </c>
       <c r="G5" s="4"/>
-      <c r="H5" s="4" t="s">
-        <v>16</v>
+      <c r="H5" s="9" t="s">
+        <v>30</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J5" s="4" t="s">
         <v>11</v>
@@ -947,20 +711,20 @@
         <v>2</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4" t="s">
-        <v>133</v>
+        <v>55</v>
       </c>
       <c r="G6" s="4"/>
-      <c r="H6" s="4" t="s">
-        <v>13</v>
+      <c r="H6" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J6" s="4" t="s">
         <v>11</v>
@@ -969,21 +733,33 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B7" s="4"/>
+      <c r="B7" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
+      <c r="F7" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
+      <c r="H7" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
@@ -4163,271 +3939,293 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G249"/>
+  <dimension ref="A1:K87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="72.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="72.42578125" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.42578125" style="7" customWidth="1"/>
     <col min="4" max="4" width="26.28515625" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.7109375" style="7" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="7"/>
-    <col min="9" max="9" width="14.28515625" style="7" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" style="7" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" style="7" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="7"/>
+    <col min="6" max="6" width="21" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="7"/>
+    <col min="12" max="12" width="11.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="B2" s="7" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="7" t="s">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="C11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="8"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D12" s="8"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B14" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C14" s="7" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
+      <c r="D14" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B15" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
+      <c r="C15" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B16" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B15" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="7" t="s">
-        <v>127</v>
-      </c>
       <c r="C16" s="7" t="s">
-        <v>19</v>
+        <v>16</v>
+      </c>
+      <c r="D16" s="7">
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B17" s="7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>130</v>
+        <v>16</v>
+      </c>
+      <c r="D17" s="7">
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B18" s="7" t="s">
-        <v>129</v>
+        <v>17</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>128</v>
+        <v>16</v>
+      </c>
+      <c r="D18" s="7">
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B19" s="7" t="s">
-        <v>127</v>
+        <v>17</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>19</v>
+        <v>16</v>
+      </c>
+      <c r="D19" s="7">
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B20" s="7" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>130</v>
+        <v>16</v>
+      </c>
+      <c r="D20" s="7">
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" s="7" t="s">
-        <v>129</v>
+        <v>17</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>128</v>
+        <v>16</v>
+      </c>
+      <c r="D21" s="7">
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B22" s="7" t="s">
-        <v>127</v>
+        <v>17</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>19</v>
+        <v>16</v>
+      </c>
+      <c r="D22" s="7">
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B23" s="7" t="s">
-        <v>91</v>
+        <v>17</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>130</v>
+        <v>16</v>
+      </c>
+      <c r="D23" s="7">
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B24" s="7" t="s">
-        <v>129</v>
+        <v>17</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>128</v>
+        <v>16</v>
+      </c>
+      <c r="D24" s="7">
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B25" s="7" t="s">
-        <v>127</v>
+        <v>17</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>19</v>
+        <v>16</v>
+      </c>
+      <c r="D25" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B26" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="7">
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="7" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B28" s="7" t="s">
+      <c r="B27" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" s="7">
         <v>23</v>
       </c>
-      <c r="C28" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>123</v>
-      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B29" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>125</v>
+      <c r="A29" s="7" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -4437,2173 +4235,439 @@
       <c r="C30" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D30" s="7" t="s">
-        <v>125</v>
-      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B31" s="7" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="C31" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B34" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D31" s="7" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B32" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C32" s="7" t="s">
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B35" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B38" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C38" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D32" s="7" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="7" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B35" s="7" t="s">
+      <c r="D38" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B39" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D39" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B40" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D40" s="7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B41" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D41" s="7">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B42" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D42" s="7">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B43" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D43" s="7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B44" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D44" s="7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B45" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D45" s="7">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B46" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D46" s="7">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B47" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D47" s="7">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B48" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D48" s="7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B49" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D49" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B50" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D50" s="7">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B51" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D51" s="7">
         <v>23</v>
       </c>
-      <c r="C35" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B36" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="C36" s="7" t="s">
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B55" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C55" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D36" s="7" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>121</v>
-      </c>
-      <c r="C38"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B39" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E39" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B40" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="E40" s="7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B41" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D41" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="E41" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B42" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D42" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="E42" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B43" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D43" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="E43" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B44" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D44" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="E44" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B45" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D45" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B46" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D46" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="E46" s="7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B47" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C47" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D47" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E47" s="7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B48" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C48" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D48" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="E48" s="7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B49" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C49" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D49" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E49" s="7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B50" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C50" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D50" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="E50" s="7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B51" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C51" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D51" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="E51" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A53" s="7" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B54" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C54" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D54" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="E54" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="F54" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="G54" s="7" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B55" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C55" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D55" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="E55" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="F55" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="G55" s="7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A57" s="7" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B58" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C58" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D58" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="E58" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="F58" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="G58" s="7" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B56" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B59" s="7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C59" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D59" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="E59" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="F59" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G59" s="7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A61" s="7" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B62" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C62" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D62" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="E62" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="F62" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="G62" s="7" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B60" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B63" s="7" t="s">
         <v>20</v>
       </c>
       <c r="C63" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D63" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="E63" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F63" s="7" t="s">
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B64" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C64" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B67" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G63" s="7" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G64" s="7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G65" s="9" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A66" s="7" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B67" s="7" t="s">
-        <v>23</v>
-      </c>
       <c r="C67" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B68" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C68" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B69" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C69" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B70" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D67" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="E67" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="F67" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="G67" s="7" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B68" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="C68" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D68" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="E68" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="F68" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="G68" s="7" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G69" s="7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G70" s="9" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A72" s="7" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B73" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C73" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D73" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="E73" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="F73" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="G73" s="7" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C70" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B71" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C71" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B74" s="7" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="C74" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D74" s="7" t="s">
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B75" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C75" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B78" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B79" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C79" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A81" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A82" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C82" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D82" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E82" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F82" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G82" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="H82" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="I82" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="J82" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="K82" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A83" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C83" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D83" s="7">
+        <v>311</v>
+      </c>
+      <c r="E83" s="7">
+        <v>300</v>
+      </c>
+      <c r="F83" s="7">
         <v>100</v>
       </c>
-      <c r="E74" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="F74" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="G74" s="7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A76" s="7" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B77" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C77" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B78" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C78" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D78" s="8"/>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B79" s="7" t="s">
+      <c r="G83" s="7">
+        <v>1000</v>
+      </c>
+      <c r="H83" s="7">
+        <v>100</v>
+      </c>
+      <c r="I83" s="7">
+        <v>150</v>
+      </c>
+      <c r="J83" s="7">
+        <v>10</v>
+      </c>
+      <c r="K83" s="7">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A85" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B86" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C79" s="7" t="s">
+      <c r="C86" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D79" s="8"/>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B80" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C80" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D80" s="8"/>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B81" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C81" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D81" s="8"/>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D82" s="8"/>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A83" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="D83" s="8"/>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B84" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C84" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D84" s="8"/>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B85" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C85" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D85" s="8"/>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D86" s="8"/>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A87" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="D87" s="8"/>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B88" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C88" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D88" s="8"/>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B89" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C89" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D89" s="8"/>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D90" s="8"/>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A91" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="D91" s="8"/>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B92" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C92" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D92" s="8"/>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B93" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C93" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D93" s="8"/>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D94" s="8"/>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A95" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="D95" s="8"/>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B96" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C96" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D96" s="8"/>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B97" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C97" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D97" s="8"/>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D98" s="8"/>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A99" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D99" s="8"/>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B100" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C100" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D100" s="8"/>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B101" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="C101" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D101" s="8"/>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D102" s="8"/>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A103" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="D103" s="8"/>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B104" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C104" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D104" s="8"/>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B105" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C105" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D105" s="8"/>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B106" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C106" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B107" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C107" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B108" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C108" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B109" s="8"/>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A110" s="8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B111" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C111" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D111" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E111" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B112" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C112" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D112" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="E112" s="7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B113" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C113" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D113" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="E113" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B114" s="8"/>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B115" s="8"/>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A116" s="8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B117" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C117" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D117" s="8"/>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B118" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C118" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D118" s="8"/>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D119" s="8"/>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A120" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="D120" s="8"/>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B121" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C121" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D121" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E121" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B122" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C122" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D122" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="E122" s="7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B123" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C123" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D123" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="E123" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B124" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C124" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D124" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="E124" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B125" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C125" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D125" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="E125" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B126" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C126" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D126" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="E126" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B127" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C127" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D127" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="E127" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B128" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C128" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D128" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="E128" s="7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B129" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C129" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D129" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E129" s="7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B130" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C130" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D130" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="E130" s="7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B131" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C131" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D131" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E131" s="7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B132" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C132" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D132" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="E132" s="7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B133" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C133" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D133" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="E133" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A135" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="D135" s="8"/>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B136" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C136" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D136" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E136" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B137" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C137" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D137" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="E137" s="7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B138" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C138" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D138" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="E138" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B139" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C139" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D139" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="E139" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B140" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C140" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D140" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="E140" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B141" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C141" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D141" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="E141" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B142" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C142" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D142" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="E142" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B143" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C143" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D143" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="E143" s="7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B144" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C144" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D144" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E144" s="7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B145" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C145" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D145" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="E145" s="7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B146" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C146" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D146" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E146" s="7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B147" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C147" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D147" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="E147" s="7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B148" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C148" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D148" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="E148" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A150" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D150" s="8"/>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B151" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C151" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D151" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B152" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C152" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D152" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B153" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C153" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D153" s="7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B154" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C154" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D154" s="7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B155" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C155" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D155" s="7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B156" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C156" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D156" s="7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B157" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C157" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D157" s="7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B158" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C158" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D158" s="7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B159" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C159" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D159" s="7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B160" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C160" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D160" s="7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B161" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C161" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D161" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B162" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C162" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D162" s="7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B163" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C163" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D163" s="7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A165" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B166" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C166" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D166" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E166" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B167" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C167" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D167" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="E167" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B168" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C168" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D168" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="E168" s="7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B169" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C169" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D169" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="E169" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B170" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C170" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D170" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="E170" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B171" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C171" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D171" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="E171" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B172" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C172" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D172" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="E172" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B173" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C173" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D173" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="E173" s="7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B174" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C174" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D174" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E174" s="7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B175" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C175" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D175" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="E175" s="7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B176" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C176" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D176" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E176" s="7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B177" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C177" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D177" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="E177" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B178" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C178" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D178" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="E178" s="7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A180" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B181" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C181" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D181" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E181" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="F181" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B182" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C182" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D182" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="E182" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="F182" s="7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B183" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C183" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D183" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="E183" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="F183" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A185" s="7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B186" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C186" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B187" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C187" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B188" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C188" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A190" s="7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B191" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C191" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D191" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B192" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C192" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D192" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B193" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C193" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D193" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B194" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C194" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D194" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B195" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C195" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D195" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A197" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B198" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C198" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D198" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E198" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F198" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B199" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C199" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D199" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="E199" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="F199" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A201" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B202" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C202" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D202" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B203" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C203" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D203" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A205" s="7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B206" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C206" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B207" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C207" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A209" s="7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B210" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C210" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D210" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E210" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F210" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="G210" s="7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B211" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C211" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D211" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E211" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F211" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="G211" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B212" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C212" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D212" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E212" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F212" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="G212" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B213" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C213" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D213" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E213" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F213" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G213" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B214" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C214" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D214" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E214" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F214" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="G214" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B215" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C215" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D215" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E215" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F215" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="G215" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A217" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B218" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C218" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D218" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B219" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C219" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D219" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A221" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B222" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C222" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D222" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B223" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C223" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D223" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A225" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B226" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C226" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B227" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C227" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B228" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C228" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A230" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B231" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C231" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D231" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B232" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C232" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D232" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B233" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C233" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D233" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B234" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C234" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D234" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B235" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C235" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D235" s="7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B236" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C236" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D236" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B237" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C237" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D237" s="7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B238" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C238" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D238" s="7">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B239" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C239" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D239" s="7">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B240" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C240" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D240" s="7">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="241" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B241" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C241" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D241" s="7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="242" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B242" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C242" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D242" s="7">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="243" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B243" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C243" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D243" s="7">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="244" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B244" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C244" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D244" s="7">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="245" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B245" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C245" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D245" s="7">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="246" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B246" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C246" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D246" s="7">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="247" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B247" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C247" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D247" s="7">
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B87" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C87" s="7" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="248" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B248" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C248" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D248" s="7">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="249" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B249" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C249" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D249" s="7">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>